<commit_message>
clean raw data files
</commit_message>
<xml_diff>
--- a/MRICloud-data.xlsx
+++ b/MRICloud-data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apenggua/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Desktop/JHU/5. Fall 2020/Compuational Medicine - Imaging/Project/GitHub/Computational-Medicine-Imaging-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BC9767-5742-B34C-82C4-94CCCF440588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB69884-F0AE-EC48-9C83-38DC258D056D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="14500" xr2:uid="{64CC52E9-E269-AA4D-B013-A553350233E9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16960" xr2:uid="{64CC52E9-E269-AA4D-B013-A553350233E9}"/>
   </bookViews>
   <sheets>
-    <sheet name="ad_zscore" sheetId="1" r:id="rId1"/>
+    <sheet name="MRI Cloud Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,82 +35,80 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t xml:space="preserve">FG_opercularis_L      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFG_orbitalis_L        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFG_triangularis_L     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFOG_L                 </t>
-  </si>
-  <si>
-    <t>MFG_L                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFOG_L                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrCG_L                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFG_L                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFG_opercularis_R      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFG_orbitalis_R        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFG_triangularis_R     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFOG_R                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFG_R                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFOG_R                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrCG_R                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFG_R                 </t>
-  </si>
-  <si>
-    <t>brain part</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ad_zscore</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>normal_zscore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>control_zscore</t>
+  </si>
+  <si>
+    <t>IFG_opercularis_L</t>
+  </si>
+  <si>
+    <t>IFG_orbitalis_L</t>
+  </si>
+  <si>
+    <t>IFG_triangularis_L</t>
+  </si>
+  <si>
+    <t>LFOG_L</t>
+  </si>
+  <si>
+    <t>MFG_L</t>
+  </si>
+  <si>
+    <t>MFOG_L</t>
+  </si>
+  <si>
+    <t>PrCG_L</t>
+  </si>
+  <si>
+    <t>SFG_L</t>
+  </si>
+  <si>
+    <t>IFG_opercularis_R</t>
+  </si>
+  <si>
+    <t>IFG_orbitalis_R</t>
+  </si>
+  <si>
+    <t>IFG_triangularis_R</t>
+  </si>
+  <si>
+    <t>LFOG_R</t>
+  </si>
+  <si>
+    <t>MFG_R</t>
+  </si>
+  <si>
+    <t>MFOG_R</t>
+  </si>
+  <si>
+    <t>PrCG_R</t>
+  </si>
+  <si>
+    <t>SFG_R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -120,7 +117,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -148,8 +145,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -160,7 +160,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -472,203 +472,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB768FC0-34F4-CF4D-BE34-F58D5C37FFA7}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="1" max="16384" width="16.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1.9922995017146801</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <v>-0.35471724942293598</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-8.4716983248765504E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-0.52030218419545604</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.30534877275716</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.52796575586537298</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.1237822605115799</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6.9270681003561103</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1.1879477956484099</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-0.30138942694535198</v>
+      </c>
+      <c r="L2" s="1">
+        <v>-0.174043636841758</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.49505144421656699</v>
+      </c>
+      <c r="N2" s="1">
+        <v>9.9672503360543292</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2.0367557648008998</v>
+      </c>
+      <c r="P2" s="1">
+        <v>-8.0965762619663706E-2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>12.9046469502468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>1.6968354898771301</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>-0.35471724942293598</v>
-      </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>-0.27519934526490603</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>-8.4716983248765504E-2</v>
-      </c>
-      <c r="C4">
+      <c r="D3" s="1">
         <v>3.8404178921392302E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>-0.52030218419545604</v>
-      </c>
-      <c r="C5">
+      <c r="E3" s="1">
         <v>-0.395575690955007</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>8.30534877275716</v>
-      </c>
-      <c r="C6">
+      <c r="F3" s="1">
         <v>7.88695869029518</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0.52796575586537298</v>
-      </c>
-      <c r="C7">
+      <c r="G3" s="1">
         <v>0.95767161443981397</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1.1237822605115799</v>
-      </c>
-      <c r="C8">
+      <c r="H3" s="1">
         <v>1.34631651460364</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>6.9270681003561103</v>
-      </c>
-      <c r="C9">
+      <c r="I3" s="1">
         <v>8.4719187678404406</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1.1879477956484099</v>
-      </c>
-      <c r="C10">
+      <c r="J3" s="1">
         <v>1.47477285754791</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>-0.30138942694535198</v>
-      </c>
-      <c r="C11">
+      <c r="K3" s="1">
         <v>-3.6665895178694799E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>-0.174043636841758</v>
-      </c>
-      <c r="C12">
+      <c r="L3" s="1">
         <v>5.0776711639061202E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0.49505144421656699</v>
-      </c>
-      <c r="C13">
+      <c r="M3" s="1">
         <v>0.848882352987269</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>9.9672503360543292</v>
-      </c>
-      <c r="C14">
+      <c r="N3" s="1">
         <v>7.9516229230654298</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>2.0367557648008998</v>
-      </c>
-      <c r="C15">
+      <c r="O3" s="1">
         <v>2.5523416274313</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>-8.0965762619663706E-2</v>
-      </c>
-      <c r="C16">
+      <c r="P3" s="1">
         <v>-4.8376373954122601E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>12.9046469502468</v>
-      </c>
-      <c r="C17">
+      <c r="Q3" s="1">
         <v>12.4289232550395</v>
       </c>
     </row>

</xml_diff>